<commit_message>
Fixed nuova Convenzione & Sfera Fix
</commit_message>
<xml_diff>
--- a/docs/tp/Sfera_4.0/NR 28.05.22/TP Quietanze scartate.xlsx
+++ b/docs/tp/Sfera_4.0/NR 28.05.22/TP Quietanze scartate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\Sfera_4.0\NR 28.05.22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C14731D-8668-4378-B72B-3DD43B2CED8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B1DCE1-C221-4EC5-95D3-1BC49853B824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="255" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="3300" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -885,41 +885,41 @@
     </row>
     <row r="16" spans="1:9" ht="38.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="9" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="13">
         <v>2</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="25.5">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="25.5">
       <c r="A18" s="3"/>

</xml_diff>